<commit_message>
Fix: Remove sample data from expense import templates.  Updated templates are now blank.
Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 32996fb4-a2c9-4212-842b-f96944ab1ce6
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/9b678722-51eb-4876-8d9c-65f766fcd8e8/b9f6b9bd-d841-486e-ac9d-07b816aeb48e.jpg
</commit_message>
<xml_diff>
--- a/static/templates/expense_import_template.xlsx
+++ b/static/templates/expense_import_template.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,156 +465,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2025-04-01</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>45.99</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Groceries</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Weekly grocery shopping</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Credit Card</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Whole Foods</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2025-04-02</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>12.5</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Transportation</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Bus fare</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Cash</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Metro Transit</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2025-04-03</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>89.98999999999999</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Entertainment</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Concert tickets</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Credit Card</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Ticketmaster</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2025-04-04</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>25.75</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Dining</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Lunch with colleagues</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Debit Card</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Cafe Bistro</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2025-04-05</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>199.99</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Shopping</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>New headphones</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Credit Card</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Electronics Store</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>